<commit_message>
Added my name to Scrum Sheet
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavanaj Biyani\Documents\CSE1325-HW6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kartik Gupta\Documents\CSE-1325-HW-6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" tabRatio="627" activeTab="1"/>
+    <workbookView xWindow="960" yWindow="0" windowWidth="19200" windowHeight="6948" tabRatio="627"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="156">
   <si>
     <t>Product Name:</t>
   </si>
@@ -484,6 +484,12 @@
   </si>
   <si>
     <t>Planning</t>
+  </si>
+  <si>
+    <t>Kartik Gupta</t>
+  </si>
+  <si>
+    <t>KG</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1279,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1308,7 +1320,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1625,25 +1643,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6328125"/>
-    <col min="2" max="2" width="13.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" style="34"/>
+    <col min="1" max="1" width="13.6640625"/>
+    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="34"/>
     <col min="4" max="4" width="11"/>
-    <col min="5" max="5" width="14.08984375" style="1"/>
-    <col min="6" max="6" width="8.1796875"/>
-    <col min="7" max="7" width="40.6328125"/>
-    <col min="8" max="8" width="41.54296875"/>
-    <col min="9" max="9" width="80.26953125"/>
-    <col min="10" max="1025" width="11.54296875"/>
+    <col min="5" max="5" width="14.109375" style="1"/>
+    <col min="6" max="6" width="8.21875"/>
+    <col min="7" max="7" width="40.6640625"/>
+    <col min="8" max="8" width="41.5546875"/>
+    <col min="9" max="9" width="80.21875"/>
+    <col min="10" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1675,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1671,7 +1689,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="33"/>
@@ -1681,7 +1699,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1695,7 +1713,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1709,7 +1727,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1723,7 +1741,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="33"/>
@@ -1733,7 +1751,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1745,11 +1763,13 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="C9" s="33"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
@@ -1757,11 +1777,13 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="C10" s="33"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
@@ -1769,11 +1791,13 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>1001228675</v>
+      </c>
       <c r="C11" s="33"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
@@ -1781,7 +1805,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12" s="3"/>
       <c r="C12" s="33"/>
@@ -1791,7 +1815,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1803,7 +1827,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1815,7 +1839,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1827,7 +1851,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16" s="3"/>
       <c r="C16" s="33"/>
@@ -1837,7 +1861,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1849,7 +1873,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1861,7 +1885,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1873,7 +1897,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20" s="3"/>
       <c r="C20" s="33"/>
@@ -1883,7 +1907,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
@@ -1902,7 +1926,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1921,7 +1945,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1941,7 +1965,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1961,7 +1985,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1981,7 +2005,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -2001,7 +2025,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -2021,7 +2045,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -2041,7 +2065,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2060,7 +2084,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="3"/>
       <c r="C30" s="33"/>
@@ -2070,7 +2094,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="3"/>
       <c r="C31" s="33"/>
@@ -2082,7 +2106,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="33"/>
@@ -2094,7 +2118,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>21</v>
       </c>
@@ -2169,7 +2193,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>3</v>
       </c>
@@ -2261,7 +2285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>7</v>
       </c>
@@ -2453,7 +2477,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="2:9" s="15" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>16</v>
       </c>
@@ -2474,7 +2498,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="2:9" s="18" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" s="18" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B50" s="16">
         <v>23</v>
       </c>
@@ -2500,7 +2524,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="2:9" s="18" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" s="18" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B51" s="16">
         <v>24</v>
       </c>
@@ -2521,7 +2545,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="2:9" s="24" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B52" s="25">
         <v>17</v>
       </c>
@@ -2542,7 +2566,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="2:9" s="24" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B53" s="25">
         <v>18</v>
       </c>
@@ -2592,7 +2616,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="2:9" s="24" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <v>22</v>
       </c>
@@ -2639,7 +2663,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="2:9" s="24" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B59" s="25">
         <v>26</v>
       </c>
@@ -2896,7 +2920,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="25" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>36</v>
       </c>
@@ -2931,23 +2955,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875"/>
-    <col min="4" max="4" width="12.26953125"/>
-    <col min="5" max="5" width="51.81640625"/>
-    <col min="6" max="6" width="11.54296875"/>
-    <col min="7" max="7" width="51.81640625"/>
-    <col min="8" max="1024" width="11.54296875"/>
+    <col min="1" max="1" width="10.21875"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875"/>
+    <col min="4" max="4" width="12.21875"/>
+    <col min="5" max="5" width="51.77734375"/>
+    <col min="6" max="6" width="11.5546875"/>
+    <col min="7" max="7" width="51.77734375"/>
+    <col min="8" max="1024" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -2962,7 +2986,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>132</v>
       </c>
@@ -2975,7 +2999,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>133</v>
       </c>
@@ -2988,7 +3012,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>134</v>
       </c>
@@ -3001,7 +3025,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="30"/>
       <c r="C5" s="2"/>
@@ -3010,7 +3034,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>135</v>
       </c>
@@ -3023,12 +3047,12 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B7" s="31">
-        <f t="shared" ref="B7:B13" si="0">B6</f>
+        <f t="shared" ref="B7:B11" si="0">B6</f>
         <v>2</v>
       </c>
       <c r="C7" s="2"/>
@@ -3037,7 +3061,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>137</v>
       </c>
@@ -3051,7 +3075,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>138</v>
       </c>
@@ -3065,7 +3089,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>139</v>
       </c>
@@ -3079,7 +3103,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>140</v>
       </c>
@@ -3093,7 +3117,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>141</v>
       </c>
@@ -3106,7 +3130,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>142</v>
       </c>
@@ -3119,7 +3143,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3128,7 +3152,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>143</v>
       </c>

</xml_diff>

<commit_message>
made changes to main.cpp (from HW 5 - use this as a model to view logic). New GUI.cpp will be the implementation file for HW 6 (DO NOT MAKE CHANGES TO THIS)
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwets_sms\Documents\CSE-1325-hw6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavanaj Biyani\Documents\CSE1325-HW6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="19200" windowHeight="6948" tabRatio="627" activeTab="1"/>
+    <workbookView xWindow="960" yWindow="0" windowWidth="19200" windowHeight="6950" tabRatio="627"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 4 Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -501,7 +501,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mmm\ dd"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
@@ -781,7 +781,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -805,7 +805,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -843,7 +842,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -886,7 +885,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FE71-4E82-BE9A-4B49D752807B}"/>
             </c:ext>
@@ -929,7 +928,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -983,7 +981,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1031,7 +1028,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -1055,7 +1052,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1093,7 +1089,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1130,7 +1126,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BE49-4C5B-90BC-2152AD412007}"/>
             </c:ext>
@@ -1173,7 +1169,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -1227,7 +1222,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1294,7 +1288,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1335,7 +1329,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1655,25 +1649,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625"/>
+    <col min="1" max="1" width="13.6328125"/>
     <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="34"/>
+    <col min="3" max="3" width="10.90625" style="34"/>
     <col min="4" max="4" width="11"/>
-    <col min="5" max="5" width="14.109375" style="1"/>
-    <col min="6" max="6" width="8.21875"/>
-    <col min="7" max="7" width="40.6640625"/>
-    <col min="8" max="8" width="41.5546875"/>
-    <col min="9" max="9" width="80.21875"/>
-    <col min="10" max="1025" width="11.5546875"/>
+    <col min="5" max="5" width="14.08984375" style="1"/>
+    <col min="6" max="6" width="8.1796875"/>
+    <col min="7" max="7" width="40.6328125"/>
+    <col min="8" max="8" width="41.54296875"/>
+    <col min="9" max="9" width="80.1796875"/>
+    <col min="10" max="1025" width="11.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1687,7 +1681,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1701,7 +1695,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="33"/>
@@ -1711,7 +1705,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1725,7 +1719,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1739,7 +1733,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1753,7 +1747,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="33"/>
@@ -1763,7 +1757,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1775,7 +1769,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1789,7 +1783,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1803,7 +1797,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1817,7 +1811,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12" s="3"/>
       <c r="C12" s="33"/>
@@ -1827,7 +1821,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1841,7 +1835,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1855,7 +1849,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1869,7 +1863,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="B16" s="3"/>
       <c r="C16" s="33"/>
@@ -1879,7 +1873,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1891,7 +1885,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1903,7 +1897,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1915,7 +1909,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20" s="3"/>
       <c r="C20" s="33"/>
@@ -1925,7 +1919,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
@@ -1944,7 +1938,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1963,7 +1957,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1983,7 +1977,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -2003,7 +1997,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2023,7 +2017,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -2043,7 +2037,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -2063,7 +2057,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -2083,7 +2077,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2102,7 +2096,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30" s="3"/>
       <c r="C30" s="33"/>
@@ -2112,7 +2106,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31" s="3"/>
       <c r="C31" s="33"/>
@@ -2124,7 +2118,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="33"/>
@@ -2136,7 +2130,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>21</v>
       </c>
@@ -2211,7 +2205,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="25" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>3</v>
       </c>
@@ -2303,7 +2297,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="25" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>7</v>
       </c>
@@ -2495,7 +2489,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="2:9" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" s="15" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>16</v>
       </c>
@@ -2516,7 +2510,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="2:9" s="18" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" s="18" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="B50" s="16">
         <v>23</v>
       </c>
@@ -2542,7 +2536,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="2:9" s="18" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" s="18" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="B51" s="16">
         <v>24</v>
       </c>
@@ -2563,7 +2557,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="2:9" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" s="24" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="B52" s="25">
         <v>17</v>
       </c>
@@ -2584,7 +2578,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="2:9" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" s="24" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="B53" s="25">
         <v>18</v>
       </c>
@@ -2634,7 +2628,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="2:9" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" s="24" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <v>22</v>
       </c>
@@ -2681,7 +2675,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="2:9" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" s="24" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="B59" s="25">
         <v>26</v>
       </c>
@@ -2938,7 +2932,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" ht="25" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>36</v>
       </c>
@@ -2973,23 +2967,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.21875"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875"/>
-    <col min="4" max="4" width="12.21875"/>
-    <col min="5" max="5" width="51.77734375"/>
-    <col min="6" max="6" width="11.5546875"/>
-    <col min="7" max="7" width="51.77734375"/>
-    <col min="8" max="1024" width="11.5546875"/>
+    <col min="1" max="1" width="10.1796875"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875"/>
+    <col min="4" max="4" width="12.1796875"/>
+    <col min="5" max="5" width="51.81640625"/>
+    <col min="6" max="6" width="11.54296875"/>
+    <col min="7" max="7" width="51.81640625"/>
+    <col min="8" max="1024" width="11.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -3004,7 +2998,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>132</v>
       </c>
@@ -3017,7 +3011,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>133</v>
       </c>
@@ -3030,7 +3024,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>134</v>
       </c>
@@ -3043,7 +3037,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="30"/>
       <c r="C5" s="2"/>
@@ -3052,7 +3046,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>135</v>
       </c>
@@ -3065,7 +3059,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>136</v>
       </c>
@@ -3079,7 +3073,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>137</v>
       </c>
@@ -3093,7 +3087,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>138</v>
       </c>
@@ -3107,7 +3101,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>139</v>
       </c>
@@ -3121,7 +3115,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>140</v>
       </c>
@@ -3135,7 +3129,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>141</v>
       </c>
@@ -3148,7 +3142,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>142</v>
       </c>
@@ -3161,7 +3155,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3170,7 +3164,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>143</v>
       </c>
@@ -3193,7 +3187,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>153</v>
       </c>
@@ -3207,7 +3201,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" ht="13.25" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>151</v>
       </c>

</xml_diff>

<commit_message>
Updated Scrum. Notice the missing features.
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="19200" windowHeight="6950" tabRatio="627" activeTab="3"/>
+    <workbookView xWindow="960" yWindow="0" windowWidth="19200" windowHeight="6950" tabRatio="627"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="177">
   <si>
     <t>Product Name:</t>
   </si>
@@ -3952,8 +3952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4736,12 +4736,6 @@
       <c r="B43" s="1">
         <v>12</v>
       </c>
-      <c r="C43" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43">
-        <v>6</v>
-      </c>
       <c r="E43" s="1">
         <v>1</v>
       </c>
@@ -4893,12 +4887,7 @@
       <c r="B49" s="15">
         <v>24</v>
       </c>
-      <c r="C49" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="17">
-        <v>6</v>
-      </c>
+      <c r="C49" s="34"/>
       <c r="E49" s="21">
         <v>2</v>
       </c>
@@ -5105,12 +5094,7 @@
       <c r="B57" s="27">
         <v>28</v>
       </c>
-      <c r="C57" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" s="26">
-        <v>6</v>
-      </c>
+      <c r="C57" s="33"/>
       <c r="E57" s="27">
         <v>4</v>
       </c>
@@ -5163,12 +5147,7 @@
       <c r="B59" s="27">
         <v>20</v>
       </c>
-      <c r="C59" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" s="26">
-        <v>6</v>
-      </c>
+      <c r="C59" s="33"/>
       <c r="E59" s="27">
         <v>4</v>
       </c>
@@ -5963,7 +5942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>